<commit_message>
Se actualizo los tooltips de las creaciones masivas para dar mejor informacion, adicionalmente se modifico el anexo 3 y se agrego un dato extra en el reporte
</commit_message>
<xml_diff>
--- a/resource/files/Anexo3.xlsx
+++ b/resource/files/Anexo3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4022DCBB-B531-4B36-911F-661D71DAD607}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Anexo3 - Listado cursos-I.U.Pas" sheetId="1" r:id="rId1"/>
@@ -22,16 +21,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>codigo</t>
+    <t>nombre</t>
   </si>
   <si>
-    <t>nombre</t>
+    <t>codigo_completo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,21 +864,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>